<commit_message>
finished files for revision E - ready for shipping
</commit_message>
<xml_diff>
--- a/hardware/tottag/rev_e/tottag_bom.xlsx
+++ b/hardware/tottag/rev_e/tottag_bom.xlsx
@@ -64,15 +64,15 @@
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
+    <t xml:space="preserve">A1,A2,A3</t>
+  </si>
+  <si>
     <t xml:space="preserve">TAIYO-YUDEN-AH086M</t>
   </si>
   <si>
     <t xml:space="preserve">N</t>
   </si>
   <si>
-    <t xml:space="preserve">A1,A2,A3</t>
-  </si>
-  <si>
     <t xml:space="preserve">UWB Antenna - 3.1-8GHz</t>
   </si>
   <si>
@@ -88,12 +88,12 @@
     <t xml:space="preserve">AH086M555003-T</t>
   </si>
   <si>
+    <t xml:space="preserve">A4</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANT3216A063R2400A</t>
   </si>
   <si>
-    <t xml:space="preserve">A4</t>
-  </si>
-  <si>
     <t xml:space="preserve">Yageo 2.4GHz</t>
   </si>
   <si>
@@ -106,21 +106,21 @@
     <t xml:space="preserve">Yageo</t>
   </si>
   <si>
+    <t xml:space="preserve">C1,C2</t>
+  </si>
+  <si>
     <t xml:space="preserve">1pF</t>
   </si>
   <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
     <t xml:space="preserve">CAPACITOR0402_CAP</t>
   </si>
   <si>
-    <t xml:space="preserve">Y</t>
-  </si>
-  <si>
     <t xml:space="preserve">0402_CAP</t>
   </si>
   <si>
-    <t xml:space="preserve">C1,C2</t>
-  </si>
-  <si>
     <t xml:space="preserve">SMD Capacitor</t>
   </si>
   <si>
@@ -136,12 +136,12 @@
     <t xml:space="preserve">500R07S1R0BV4T</t>
   </si>
   <si>
+    <t xml:space="preserve">C3</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.2pF</t>
   </si>
   <si>
-    <t xml:space="preserve">C3</t>
-  </si>
-  <si>
     <t xml:space="preserve">CAP CER 1.2PF 50V C0G/NP0 0402</t>
   </si>
   <si>
@@ -154,12 +154,12 @@
     <t xml:space="preserve">GJM1555C1H1R2CB01D</t>
   </si>
   <si>
+    <t xml:space="preserve">C4,C5</t>
+  </si>
+  <si>
     <t xml:space="preserve">10pF</t>
   </si>
   <si>
-    <t xml:space="preserve">C4,C5</t>
-  </si>
-  <si>
     <t xml:space="preserve">CAP CER 10PF 100V C0G/NP0 0402</t>
   </si>
   <si>
@@ -169,6 +169,9 @@
     <t xml:space="preserve">Wurth Electronics Inc.</t>
   </si>
   <si>
+    <t xml:space="preserve">C6,C7</t>
+  </si>
+  <si>
     <t xml:space="preserve">12pF</t>
   </si>
   <si>
@@ -178,9 +181,6 @@
     <t xml:space="preserve">0201_CAP</t>
   </si>
   <si>
-    <t xml:space="preserve">C6,C7</t>
-  </si>
-  <si>
     <t xml:space="preserve">CAP CER 12PF 25V C0G/NP0 0201</t>
   </si>
   <si>
@@ -202,141 +202,141 @@
     <t xml:space="preserve">GJM1555C1H120FB01D</t>
   </si>
   <si>
+    <t xml:space="preserve">C16</t>
+  </si>
+  <si>
     <t xml:space="preserve">18pF</t>
   </si>
   <si>
-    <t xml:space="preserve">C16</t>
-  </si>
-  <si>
     <t xml:space="preserve">CAP CER 18PF 50V C0G/NP0 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">490-14582-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRM1555C1H180JA01J</t>
+    <t xml:space="preserve">399-8828-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KEMET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CBR04C180F5GAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C17</t>
   </si>
   <si>
     <t xml:space="preserve">27pF</t>
   </si>
   <si>
-    <t xml:space="preserve">C17</t>
-  </si>
-  <si>
     <t xml:space="preserve">CAP CER 27PF 50V C0G/NP0 0402</t>
   </si>
   <si>
-    <t xml:space="preserve">1276-1153-1-ND</t>
+    <t xml:space="preserve">490-16380-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GJM1555C1H270FB01D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100pF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP CER SMD 0402 100PF 5% X7R 50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">399-17545-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C0402C101J5RACAUTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C19,C20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">330pF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP CER 330PF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-3768-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC0402JRX7R9BB331</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C21,C22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">820pF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP CER 820PF 25V NP0 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">399-15345-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C0402C821J3GAC7867</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C23,C24,C25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10nF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP CER 10000PF 25V X7R 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">399-1279-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C0402C103J3RACTU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47nF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP CER 0.047UF 16V X7R 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">445-1264-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TDK Corporation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1005X7R1C473K050BC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C27,C28,C29,C30,C31,C32,C33,C34,C35,C36,C37,C38,C39,C40,C41,C42,C43,C44,C45,C46,C47,C48,C49,C50,C51,C52,C53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAP CER 0.1UF 16V X5R 0402</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1276-1234-1-ND</t>
   </si>
   <si>
     <t xml:space="preserve">Samsung Electro-Mechanics</t>
   </si>
   <si>
-    <t xml:space="preserve">CL05C270JB5NNNC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100pF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAP CER SMD 0402 100PF 5% X7R 50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">399-17545-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KEMET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C0402C101J5RACAUTO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">330pF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C19,C20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAP CER 330PF 50V X7R 0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">311-3768-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC0402JRX7R9BB331</t>
-  </si>
-  <si>
-    <t xml:space="preserve">820pF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C21,C22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MLCC 1005(0402) C0G 820PF 5% 50V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1276-6989-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CL05C821JB5NFNC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10nF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C23,C24,C25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAP CER 10000PF 25V X7R 0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">399-1279-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C0402C103J3RACTU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47nF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAP CER 0.047UF 16V X7R 0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">445-1264-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TDK Corporation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C1005X7R1C473K050BC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1uF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C27,C28,C29,C30,C31,C32,C33,C34,C35,C36,C37,C38,C39,C40,C41,C42,C43,C44,C45,C46,C47,C48,C49,C50,C51,C52,C53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAP CER 0.1UF 16V X5R 0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1276-1234-1-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">CL05A104KO5NNNC</t>
   </si>
   <si>
+    <t xml:space="preserve">C54,C55,C56,C57</t>
+  </si>
+  <si>
     <t xml:space="preserve">1uF</t>
   </si>
   <si>
-    <t xml:space="preserve">C54,C55,C56,C57</t>
-  </si>
-  <si>
     <t xml:space="preserve">CAP CER 1UF 10V X6S 0402</t>
   </si>
   <si>
@@ -346,12 +346,12 @@
     <t xml:space="preserve">CL05X105KP5NNNC</t>
   </si>
   <si>
+    <t xml:space="preserve">C58,C59,C60,C61,C62,C63,C64,C65,C66,C67,C68</t>
+  </si>
+  <si>
     <t xml:space="preserve">4.7uF</t>
   </si>
   <si>
-    <t xml:space="preserve">C58,C59,C60,C61,C62,C63,C64,C65,C66,C67,C68</t>
-  </si>
-  <si>
     <t xml:space="preserve">CAP CER 4.7UF 10V X5R 0402</t>
   </si>
   <si>
@@ -361,6 +361,9 @@
     <t xml:space="preserve">GRM155R61A475MEAAD</t>
   </si>
   <si>
+    <t xml:space="preserve">C69,C70</t>
+  </si>
+  <si>
     <t xml:space="preserve">10uF</t>
   </si>
   <si>
@@ -370,9 +373,6 @@
     <t xml:space="preserve">0603_CAP</t>
   </si>
   <si>
-    <t xml:space="preserve">C69,C70</t>
-  </si>
-  <si>
     <t xml:space="preserve">CAP CER 10UF 10V X5R 0603</t>
   </si>
   <si>
@@ -382,12 +382,12 @@
     <t xml:space="preserve">GRM188R61A106KE69D</t>
   </si>
   <si>
+    <t xml:space="preserve">C71</t>
+  </si>
+  <si>
     <t xml:space="preserve">47uF</t>
   </si>
   <si>
-    <t xml:space="preserve">C71</t>
-  </si>
-  <si>
     <t xml:space="preserve">CAP CER 47UF 6.3V X5R 0603</t>
   </si>
   <si>
@@ -400,6 +400,9 @@
     <t xml:space="preserve">81-GRM188R60J476ME5D</t>
   </si>
   <si>
+    <t xml:space="preserve">D1</t>
+  </si>
+  <si>
     <t xml:space="preserve">GREEN</t>
   </si>
   <si>
@@ -409,9 +412,6 @@
     <t xml:space="preserve">LED-0603</t>
   </si>
   <si>
-    <t xml:space="preserve">D1</t>
-  </si>
-  <si>
     <t xml:space="preserve">LED (Generic)</t>
   </si>
   <si>
@@ -427,15 +427,15 @@
     <t xml:space="preserve">LTST-C191KGKT</t>
   </si>
   <si>
+    <t xml:space="preserve">D2,D3</t>
+  </si>
+  <si>
     <t xml:space="preserve">SML-LX0404SIUPGUSB</t>
   </si>
   <si>
     <t xml:space="preserve">1MM_SQ_4PAD</t>
   </si>
   <si>
-    <t xml:space="preserve">D2,D3</t>
-  </si>
-  <si>
     <t xml:space="preserve">1mm^2 RGB LED</t>
   </si>
   <si>
@@ -448,15 +448,15 @@
     <t xml:space="preserve">Lumex Opto/Components Inc.</t>
   </si>
   <si>
+    <t xml:space="preserve">J1</t>
+  </si>
+  <si>
     <t xml:space="preserve">MICRO_USB_B_HIROSE_ZX62-B-5PA(11)</t>
   </si>
   <si>
     <t xml:space="preserve">USB_MICRO_B-HIROSE-ZX62-B-5PA(11)</t>
   </si>
   <si>
-    <t xml:space="preserve">J1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Connector Receptacle USB - micro B 2.0 5 Position Surface Mount, Right Angle, Horizontal</t>
   </si>
   <si>
@@ -472,12 +472,12 @@
     <t xml:space="preserve">DM3AT-SF-PEJM5</t>
   </si>
   <si>
+    <t xml:space="preserve">J2</t>
+  </si>
+  <si>
     <t xml:space="preserve">CON_MICRO_SDDM3AT-SF-PEJM5</t>
   </si>
   <si>
-    <t xml:space="preserve">J2</t>
-  </si>
-  <si>
     <t xml:space="preserve">CONN MICRO SD R/A PUSH-PUSH SMD</t>
   </si>
   <si>
@@ -490,15 +490,15 @@
     <t xml:space="preserve">ZX62-B-5PA(33)</t>
   </si>
   <si>
+    <t xml:space="preserve">L1</t>
+  </si>
+  <si>
     <t xml:space="preserve">3.9nH</t>
   </si>
   <si>
     <t xml:space="preserve">INDUCTOR0402</t>
   </si>
   <si>
-    <t xml:space="preserve">L1</t>
-  </si>
-  <si>
     <t xml:space="preserve">A very specific inductor</t>
   </si>
   <si>
@@ -514,12 +514,12 @@
     <t xml:space="preserve">AISC-0402-3N9G-T</t>
   </si>
   <si>
+    <t xml:space="preserve">L2</t>
+  </si>
+  <si>
     <t xml:space="preserve">15nH</t>
   </si>
   <si>
-    <t xml:space="preserve">L2</t>
-  </si>
-  <si>
     <t xml:space="preserve">FIXED IND 15NH 320MA 460 MOHM</t>
   </si>
   <si>
@@ -529,15 +529,15 @@
     <t xml:space="preserve">HK100515NJ-T</t>
   </si>
   <si>
+    <t xml:space="preserve">L3</t>
+  </si>
+  <si>
     <t xml:space="preserve">10uH</t>
   </si>
   <si>
     <t xml:space="preserve">INDUCTOR0603</t>
   </si>
   <si>
-    <t xml:space="preserve">L3</t>
-  </si>
-  <si>
     <t xml:space="preserve">FIXED IND 10UH 300MA 600 MOHM</t>
   </si>
   <si>
@@ -547,15 +547,15 @@
     <t xml:space="preserve">MLZ1608N100LT000</t>
   </si>
   <si>
+    <t xml:space="preserve">R1,R2</t>
+  </si>
+  <si>
     <t xml:space="preserve">RESISTOR0402_RES</t>
   </si>
   <si>
     <t xml:space="preserve">0402_RES</t>
   </si>
   <si>
-    <t xml:space="preserve">R1,R2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Resistor</t>
   </si>
   <si>
@@ -598,12 +598,12 @@
     <t xml:space="preserve">CRCW0402470RFKEDC</t>
   </si>
   <si>
+    <t xml:space="preserve">R7,R8,R9,R10</t>
+  </si>
+  <si>
     <t xml:space="preserve">1k</t>
   </si>
   <si>
-    <t xml:space="preserve">R7,R8,R9,R10</t>
-  </si>
-  <si>
     <t xml:space="preserve">RES SMD 1K OHM 1% 1/5W 0402</t>
   </si>
   <si>
@@ -613,12 +613,12 @@
     <t xml:space="preserve">RCA04021K00FKEDHP</t>
   </si>
   <si>
+    <t xml:space="preserve">R11</t>
+  </si>
+  <si>
     <t xml:space="preserve">2k 1%</t>
   </si>
   <si>
-    <t xml:space="preserve">R11</t>
-  </si>
-  <si>
     <t xml:space="preserve">RES SMD 2K OHM 1% 1/10W 0402</t>
   </si>
   <si>
@@ -628,12 +628,12 @@
     <t xml:space="preserve">ERJ-2RKF2001X</t>
   </si>
   <si>
+    <t xml:space="preserve">R12,R13,R14</t>
+  </si>
+  <si>
     <t xml:space="preserve">10k</t>
   </si>
   <si>
-    <t xml:space="preserve">R12,R13,R14</t>
-  </si>
-  <si>
     <t xml:space="preserve">RES SMD 10K OHM 5% 1/10W 0402</t>
   </si>
   <si>
@@ -643,12 +643,12 @@
     <t xml:space="preserve">ERJ-2GEJ103X</t>
   </si>
   <si>
+    <t xml:space="preserve">R15,R16</t>
+  </si>
+  <si>
     <t xml:space="preserve">11k 1%</t>
   </si>
   <si>
-    <t xml:space="preserve">R15,R16</t>
-  </si>
-  <si>
     <t xml:space="preserve">RES SMD 11K OHM 1% 1/10W 0402</t>
   </si>
   <si>
@@ -658,12 +658,12 @@
     <t xml:space="preserve">ERJ-2RKF1102X</t>
   </si>
   <si>
+    <t xml:space="preserve">R17</t>
+  </si>
+  <si>
     <t xml:space="preserve">16k</t>
   </si>
   <si>
-    <t xml:space="preserve">R17</t>
-  </si>
-  <si>
     <t xml:space="preserve">RES SMD 16K OHM 1% 1/16W 0402</t>
   </si>
   <si>
@@ -673,12 +673,12 @@
     <t xml:space="preserve">AC0402FR-0716KL</t>
   </si>
   <si>
+    <t xml:space="preserve">R18,R19,R20</t>
+  </si>
+  <si>
     <t xml:space="preserve">100k</t>
   </si>
   <si>
-    <t xml:space="preserve">R18,R19,R20</t>
-  </si>
-  <si>
     <t xml:space="preserve">RES SMD 100K OHM 1% 1/16W 0402</t>
   </si>
   <si>
@@ -688,12 +688,12 @@
     <t xml:space="preserve">CRCW0402100KFKEDC</t>
   </si>
   <si>
+    <t xml:space="preserve">R21</t>
+  </si>
+  <si>
     <t xml:space="preserve">2.2M</t>
   </si>
   <si>
-    <t xml:space="preserve">R21</t>
-  </si>
-  <si>
     <t xml:space="preserve">RES SMD 2.2M OHM 1% 1/16W 0402</t>
   </si>
   <si>
@@ -703,12 +703,12 @@
     <t xml:space="preserve">CRCW04022M20FKEDC</t>
   </si>
   <si>
+    <t xml:space="preserve">R22</t>
+  </si>
+  <si>
     <t xml:space="preserve">10M</t>
   </si>
   <si>
-    <t xml:space="preserve">R22</t>
-  </si>
-  <si>
     <t xml:space="preserve">RES SMD 10M OHM 5% 1/10W 0402</t>
   </si>
   <si>
@@ -718,15 +718,15 @@
     <t xml:space="preserve">ERJ-2GEJ106X</t>
   </si>
   <si>
+    <t xml:space="preserve">T1</t>
+  </si>
+  <si>
     <t xml:space="preserve">HHM1595A1</t>
   </si>
   <si>
     <t xml:space="preserve">EIA-0805</t>
   </si>
   <si>
-    <t xml:space="preserve">T1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Description: Symbol for HHM1595A1, a multilayer Balun from TDK.</t>
   </si>
   <si>
@@ -736,15 +736,15 @@
     <t xml:space="preserve">445-3387-1-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">U1</t>
+  </si>
+  <si>
     <t xml:space="preserve">DW1000</t>
   </si>
   <si>
     <t xml:space="preserve">QFN-48-DW1000</t>
   </si>
   <si>
-    <t xml:space="preserve">U1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Description: The DecaWave DW1000 chip, used for UWB two-way ranging.</t>
   </si>
   <si>
@@ -760,15 +760,195 @@
     <t xml:space="preserve">DW1000-I-TR13</t>
   </si>
   <si>
+    <t xml:space="preserve">U2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FT232RQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QFN32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source: http://www.ftdichip.com/Documents/DataSheets/DS_FT232R_v104.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC USB FS SERIAL UART 32-QFN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">768-1008-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FTDI, Future Technology Devices International Ltd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIS2DW12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LGA-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ultra low power 3 axis accelerometer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEMS DIGITAL OUTPUT MOTION SENSOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">497-17718-6-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STMicroelectronics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIS2DW12TR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LXDC2HN18A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LXDC2HN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description: Symbol for LXDC2HN18A-097, a DC-DC converter by Murata Electronics.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DC/DC CONVERTER SMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">490-12092-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LXDC2HN18A-097</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAX8887EZK33+T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOT-23-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC REG LDO 3.3V 0.3A TSOT23-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC REG LIN 3.3V 300MA TSOT23-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAX8887EZK33+TCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maxim Integrated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCP73831</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DFN-8-MCP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description: Device for MCP73831, a battery charge controller from Microchip.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC CONTROLLER LI-ION 4.2V 8DFN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCP73831T-2ACI/MCCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microchip Technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCP73831T-2ACI/MC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NRF52840</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AQFN73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ultra-low power 2.4 GHz wireless system on chip (SoC) integrating a multiprotocol 2.4 GHz transceiver, an ARM® Cortex®-M4F CPU.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NRF52840-QIAA QFN 73L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1490-1071-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nordic Semiconductor ASA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIP32510</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSOT23-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load switch, slew rate controlled. By Vishay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC LOAD SWITCH SOT23-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SIP32510DT-T1-GE3CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vishay Siliconix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIP32510DT-T1-GE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKY13317</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MLPQ-UT-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description: Device for SKY13317-373LF, an RF switch from Skyworks Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC SWITCH RF SP3T 8-MLP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">863-1056-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skyworks Solutions Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKY13317-373LF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U10</t>
+  </si>
+  <si>
     <t xml:space="preserve">STM32F091CC</t>
   </si>
   <si>
     <t xml:space="preserve">UFQFPN-48</t>
   </si>
   <si>
-    <t xml:space="preserve">U10</t>
-  </si>
-  <si>
     <t xml:space="preserve">Description: STM32F091CC from STMicroelectronics, an ARM-based 32-bit MCU with 256 kB Flash, 32kB of SRAM and a Cortex M0</t>
   </si>
   <si>
@@ -778,187 +958,10 @@
     <t xml:space="preserve">497-15813-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">STMicroelectronics</t>
-  </si>
-  <si>
     <t xml:space="preserve">STM32F091CCU6</t>
   </si>
   <si>
-    <t xml:space="preserve">FT232RQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QFN32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source: http://www.ftdichip.com/Documents/DataSheets/DS_FT232R_v104.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC USB FS SERIAL UART 32-QFN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">768-1008-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FTDI, Future Technology Devices International Ltd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIS2DW12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LGA-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ultra low power 3 axis accelerometer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MEMS DIGITAL OUTPUT MOTION SENSOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">497-17718-6-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LIS2DW12TR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LXDC2HN18A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LXDC2HN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description: Symbol for LXDC2HN18A-097, a DC-DC converter by Murata Electronics.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DC/DC CONVERTER SMD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">490-12092-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LXDC2HN18A-097</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAX8887EZK33+T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOT-23-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC REG LDO 3.3V 0.3A TSOT23-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC REG LIN 3.3V 300MA TSOT23-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAX8887EZK33+TCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maxim Integrated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCP73831</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DFN-8-MCP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description: Device for MCP73831, a battery charge controller from Microchip.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC CONTROLLER LI-ION 4.2V 8DFN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCP73831T-2ACI/MCCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Microchip Technology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCP73831T-2ACI/MC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NRF52840</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AQFN73</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ultra-low power 2.4 GHz wireless system on chip (SoC) integrating a multiprotocol 2.4 GHz transceiver, an ARM® Cortex®-M4F CPU.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NRF52840-QIAA QFN 73L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1490-1071-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nordic Semiconductor ASA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIP32510</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TSOT23-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Load switch, slew rate controlled. By Vishay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC LOAD SWITCH SOT23-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SIP32510DT-T1-GE3CT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vishay Siliconix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIP32510DT-T1-GE3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKY13317</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MLPQ-UT-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description: Device for SKY13317-373LF, an RF switch from Skyworks Inc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC SWITCH RF SP3T 8-MLP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">863-1056-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Skyworks Solutions Inc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKY13317-373LF</t>
+    <t xml:space="preserve">X1</t>
   </si>
   <si>
     <t xml:space="preserve">32.768kHz</t>
@@ -970,9 +973,6 @@
     <t xml:space="preserve">ABS05</t>
   </si>
   <si>
-    <t xml:space="preserve">X1</t>
-  </si>
-  <si>
     <t xml:space="preserve">32.768kHz Crystal</t>
   </si>
   <si>
@@ -982,15 +982,15 @@
     <t xml:space="preserve">535-11897-1-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">X2</t>
+  </si>
+  <si>
     <t xml:space="preserve">16MHz</t>
   </si>
   <si>
     <t xml:space="preserve">FA-20H</t>
   </si>
   <si>
-    <t xml:space="preserve">X2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Description: Oscillator by EPSON from 12MHz to 54 MHz</t>
   </si>
   <si>
@@ -1006,6 +1006,9 @@
     <t xml:space="preserve">FA-20H 16.0000MF10Z-AJ5</t>
   </si>
   <si>
+    <t xml:space="preserve">X3</t>
+  </si>
+  <si>
     <t xml:space="preserve">32MHz</t>
   </si>
   <si>
@@ -1015,9 +1018,6 @@
     <t xml:space="preserve">TXC-7V</t>
   </si>
   <si>
-    <t xml:space="preserve">X3</t>
-  </si>
-  <si>
     <t xml:space="preserve">TXC CRYSTAL SMD</t>
   </si>
   <si>
@@ -1033,12 +1033,12 @@
     <t xml:space="preserve">7M-32.000MAHV-T</t>
   </si>
   <si>
+    <t xml:space="preserve">X4</t>
+  </si>
+  <si>
     <t xml:space="preserve">38.4MHz</t>
   </si>
   <si>
-    <t xml:space="preserve">X4</t>
-  </si>
-  <si>
     <t xml:space="preserve">38.4MHz ±10ppm Crystal 8.5pF 40 Ohms 4-SMD, No Lead</t>
   </si>
   <si>
@@ -1048,6 +1048,9 @@
     <t xml:space="preserve">FA-20H 38.4000MF10Z-AS3</t>
   </si>
   <si>
+    <t xml:space="preserve">+1V8,MISO,MOSI,SPI_CLK,TP1,TP2,TP3,TP4,TP15</t>
+  </si>
+  <si>
     <t xml:space="preserve">TPTP06SQ</t>
   </si>
   <si>
@@ -1057,19 +1060,19 @@
     <t xml:space="preserve">TP06SQ</t>
   </si>
   <si>
-    <t xml:space="preserve">+1V8,MISO,MOSI,SPI_CLK,TP1,TP2,TP3,TP4,TP15</t>
-  </si>
-  <si>
     <t xml:space="preserve">Test pad</t>
   </si>
   <si>
+    <t xml:space="preserve">GPIO0,GPIO1,TP5,TP6,TP7,TP8,TP9,TP10,TP11,TP12,TP13,TP14</t>
+  </si>
+  <si>
     <t xml:space="preserve">TEST-POINT</t>
   </si>
   <si>
     <t xml:space="preserve">PAD.03X.03</t>
   </si>
   <si>
-    <t xml:space="preserve">GPIO0,GPIO1,TP5,TP6,TP7,TP8,TP9,TP10,TP11,TP12,TP13,TP14</t>
+    <t xml:space="preserve">J3</t>
   </si>
   <si>
     <t xml:space="preserve">BAT_HOLE</t>
@@ -1078,7 +1081,7 @@
     <t xml:space="preserve">BATTERY_HOLE</t>
   </si>
   <si>
-    <t xml:space="preserve">J3</t>
+    <t xml:space="preserve">J4,J5</t>
   </si>
   <si>
     <t xml:space="preserve">TC2030-JLINK-NL</t>
@@ -1087,16 +1090,13 @@
     <t xml:space="preserve">TC2030-IDC-NL</t>
   </si>
   <si>
-    <t xml:space="preserve">J4,J5</t>
+    <t xml:space="preserve">JP1</t>
   </si>
   <si>
     <t xml:space="preserve">JUMPER-SMT_2_NO_NO-SILK</t>
   </si>
   <si>
     <t xml:space="preserve">SMT-JUMPER_2_NO_NO-SILK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JP1</t>
   </si>
   <si>
     <t xml:space="preserve">Normally open jumper</t>
@@ -1109,7 +1109,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1141,13 +1141,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCE181E"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1216,7 +1209,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1259,10 +1252,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1375,7 +1364,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FFCE181E"/>
+      <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -1391,8 +1380,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K57" activeCellId="0" sqref="K57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M30" activeCellId="0" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1402,14 +1391,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="95.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="74.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="62.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="41.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="28.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="33.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="59.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="27.28"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="11.52"/>
   </cols>
@@ -1471,17 +1460,17 @@
         <v>14</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>17</v>
@@ -1508,14 +1497,14 @@
         <v>22</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>23</v>
@@ -1533,7 +1522,7 @@
         <v>27</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N3" s="0"/>
     </row>
@@ -1582,17 +1571,17 @@
         <v>38</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="0" t="s">
         <v>31</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>33</v>
@@ -1619,7 +1608,7 @@
         <v>44</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>30</v>
@@ -1629,7 +1618,7 @@
         <v>31</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>33</v>
@@ -1659,7 +1648,7 @@
         <v>50</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="0" t="s">
@@ -1689,21 +1678,21 @@
       <c r="A8" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>49</v>
+      <c r="B8" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>56</v>
+      <c r="G8" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>33</v>
@@ -1730,17 +1719,17 @@
         <v>60</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="0" t="s">
         <v>31</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>33</v>
@@ -1752,10 +1741,10 @@
         <v>63</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N9" s="0"/>
     </row>
@@ -1764,32 +1753,32 @@
         <v>1</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="0" t="s">
         <v>31</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>33</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="L10" s="0" t="s">
         <v>70</v>
@@ -1804,7 +1793,7 @@
         <v>71</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>30</v>
@@ -1814,7 +1803,7 @@
         <v>31</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="H11" s="0" t="s">
         <v>33</v>
@@ -1826,10 +1815,10 @@
         <v>74</v>
       </c>
       <c r="K11" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="L11" s="0" t="s">
         <v>75</v>
-      </c>
-      <c r="L11" s="0" t="s">
-        <v>76</v>
       </c>
       <c r="N11" s="0"/>
     </row>
@@ -1838,10 +1827,10 @@
         <v>2</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>77</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>30</v>
@@ -1851,22 +1840,22 @@
         <v>31</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>33</v>
       </c>
       <c r="I12" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="J12" s="9" t="s">
         <v>79</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>80</v>
       </c>
       <c r="K12" s="0" t="s">
         <v>27</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N12" s="0"/>
     </row>
@@ -1875,35 +1864,35 @@
         <v>2</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="D13" s="5" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="0" t="s">
         <v>31</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>83</v>
+        <v>32</v>
       </c>
       <c r="H13" s="0" t="s">
         <v>33</v>
       </c>
       <c r="I13" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="J13" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="J13" s="9" t="s">
+      <c r="K13" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="L13" s="0" t="s">
         <v>85</v>
-      </c>
-      <c r="K13" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="L13" s="0" t="s">
-        <v>86</v>
       </c>
       <c r="N13" s="0"/>
     </row>
@@ -1912,10 +1901,10 @@
         <v>3</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>87</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>30</v>
@@ -1925,22 +1914,22 @@
         <v>31</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>88</v>
+        <v>32</v>
       </c>
       <c r="H14" s="0" t="s">
         <v>33</v>
       </c>
       <c r="I14" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="J14" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="J14" s="9" t="s">
+      <c r="K14" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="L14" s="0" t="s">
         <v>90</v>
-      </c>
-      <c r="K14" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="L14" s="0" t="s">
-        <v>91</v>
       </c>
       <c r="N14" s="0"/>
     </row>
@@ -1949,10 +1938,10 @@
         <v>1</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>92</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>30</v>
@@ -1962,22 +1951,22 @@
         <v>31</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="H15" s="0" t="s">
         <v>33</v>
       </c>
       <c r="I15" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="J15" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="J15" s="9" t="s">
+      <c r="K15" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="K15" s="0" t="s">
+      <c r="L15" s="0" t="s">
         <v>96</v>
-      </c>
-      <c r="L15" s="0" t="s">
-        <v>97</v>
       </c>
       <c r="N15" s="0"/>
     </row>
@@ -1986,10 +1975,10 @@
         <v>27</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="0" t="s">
         <v>98</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>29</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>30</v>
@@ -1999,19 +1988,19 @@
         <v>31</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="H16" s="0" t="s">
         <v>33</v>
       </c>
       <c r="I16" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="J16" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="J16" s="9" t="s">
+      <c r="K16" s="0" t="s">
         <v>101</v>
-      </c>
-      <c r="K16" s="0" t="s">
-        <v>69</v>
       </c>
       <c r="L16" s="0" t="s">
         <v>102</v>
@@ -2026,7 +2015,7 @@
         <v>103</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>30</v>
@@ -2036,7 +2025,7 @@
         <v>31</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>104</v>
+        <v>32</v>
       </c>
       <c r="H17" s="0" t="s">
         <v>33</v>
@@ -2048,7 +2037,7 @@
         <v>106</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>69</v>
+        <v>101</v>
       </c>
       <c r="L17" s="0" t="s">
         <v>107</v>
@@ -2063,7 +2052,7 @@
         <v>108</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>30</v>
@@ -2073,7 +2062,7 @@
         <v>31</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>109</v>
+        <v>32</v>
       </c>
       <c r="H18" s="0" t="s">
         <v>33</v>
@@ -2137,7 +2126,7 @@
         <v>120</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>30</v>
@@ -2147,7 +2136,7 @@
         <v>115</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="H20" s="0" t="s">
         <v>33</v>
@@ -2214,7 +2203,7 @@
         <v>135</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>30</v>
@@ -2239,7 +2228,7 @@
         <v>141</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="N22" s="0"/>
     </row>
@@ -2251,10 +2240,10 @@
         <v>142</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="0" t="s">
@@ -2288,17 +2277,17 @@
         <v>150</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="G24" s="0" t="s">
         <v>149</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>151</v>
       </c>
       <c r="H24" s="0" t="s">
         <v>152</v>
@@ -2332,10 +2321,10 @@
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="0" t="s">
-        <v>31</v>
+        <v>158</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>158</v>
+        <v>32</v>
       </c>
       <c r="H25" s="0" t="s">
         <v>159</v>
@@ -2362,17 +2351,17 @@
         <v>164</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>30</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="0" t="s">
-        <v>31</v>
+        <v>158</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>165</v>
+        <v>32</v>
       </c>
       <c r="H26" s="0" t="s">
         <v>159</v>
@@ -2406,10 +2395,10 @@
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="0" t="s">
-        <v>115</v>
+        <v>171</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>171</v>
+        <v>116</v>
       </c>
       <c r="H27" s="0" t="s">
         <v>159</v>
@@ -2421,7 +2410,7 @@
         <v>173</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L27" s="0" t="s">
         <v>174</v>
@@ -2432,11 +2421,11 @@
       <c r="A28" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B28" s="8" t="n">
+      <c r="B28" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="C28" s="8" t="n">
         <v>0</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>175</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>30</v>
@@ -2469,21 +2458,21 @@
       <c r="A29" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B29" s="8" t="n">
+      <c r="B29" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="C29" s="8" t="n">
         <v>270</v>
       </c>
-      <c r="C29" s="0" t="s">
-        <v>175</v>
-      </c>
       <c r="D29" s="5" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="0" t="s">
         <v>176</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="H29" s="0" t="s">
         <v>178</v>
@@ -2495,7 +2484,7 @@
         <v>185</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>69</v>
+        <v>101</v>
       </c>
       <c r="L29" s="0" t="s">
         <v>186</v>
@@ -2506,11 +2495,11 @@
       <c r="A30" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B30" s="8" t="n">
+      <c r="B30" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="C30" s="8" t="n">
         <v>470</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>175</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>30</v>
@@ -2520,7 +2509,7 @@
         <v>176</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="H30" s="0" t="s">
         <v>178</v>
@@ -2547,7 +2536,7 @@
         <v>192</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>175</v>
+        <v>193</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>30</v>
@@ -2557,7 +2546,7 @@
         <v>176</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="H31" s="0" t="s">
         <v>178</v>
@@ -2584,7 +2573,7 @@
         <v>197</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>175</v>
+        <v>198</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>30</v>
@@ -2594,7 +2583,7 @@
         <v>176</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="H32" s="0" t="s">
         <v>178</v>
@@ -2621,7 +2610,7 @@
         <v>202</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>175</v>
+        <v>203</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>30</v>
@@ -2631,7 +2620,7 @@
         <v>176</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>203</v>
+        <v>177</v>
       </c>
       <c r="H33" s="0" t="s">
         <v>178</v>
@@ -2658,7 +2647,7 @@
         <v>207</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>175</v>
+        <v>208</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>30</v>
@@ -2668,7 +2657,7 @@
         <v>176</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>208</v>
+        <v>177</v>
       </c>
       <c r="H34" s="0" t="s">
         <v>178</v>
@@ -2695,17 +2684,17 @@
         <v>212</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>175</v>
+        <v>213</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="0" t="s">
         <v>176</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>213</v>
+        <v>177</v>
       </c>
       <c r="H35" s="0" t="s">
         <v>178</v>
@@ -2732,7 +2721,7 @@
         <v>217</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>175</v>
+        <v>218</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>30</v>
@@ -2742,7 +2731,7 @@
         <v>176</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>218</v>
+        <v>177</v>
       </c>
       <c r="H36" s="0" t="s">
         <v>178</v>
@@ -2769,7 +2758,7 @@
         <v>222</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>175</v>
+        <v>223</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>30</v>
@@ -2779,7 +2768,7 @@
         <v>176</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="H37" s="0" t="s">
         <v>178</v>
@@ -2806,7 +2795,7 @@
         <v>227</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>175</v>
+        <v>228</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>30</v>
@@ -2816,7 +2805,7 @@
         <v>176</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>228</v>
+        <v>177</v>
       </c>
       <c r="H38" s="0" t="s">
         <v>178</v>
@@ -2843,10 +2832,10 @@
         <v>232</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E39" s="6"/>
       <c r="F39" s="0" t="s">
@@ -2865,10 +2854,10 @@
         <v>237</v>
       </c>
       <c r="K39" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L39" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="N39" s="0"/>
     </row>
@@ -2880,10 +2869,10 @@
         <v>238</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E40" s="6"/>
       <c r="F40" s="0" t="s">
@@ -2917,10 +2906,10 @@
         <v>246</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E41" s="6"/>
       <c r="F41" s="0" t="s">
@@ -2942,7 +2931,7 @@
         <v>252</v>
       </c>
       <c r="L41" s="0" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="N41" s="0"/>
     </row>
@@ -2951,35 +2940,35 @@
         <v>1</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>254</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E42" s="6"/>
       <c r="F42" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="G42" s="0" t="s">
         <v>255</v>
       </c>
-      <c r="G42" s="0" t="s">
+      <c r="H42" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="H42" s="0" t="s">
+      <c r="I42" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="I42" s="0" t="s">
+      <c r="J42" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="J42" s="0" t="s">
+      <c r="K42" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="K42" s="0" t="s">
+      <c r="L42" s="0" t="s">
         <v>260</v>
-      </c>
-      <c r="L42" s="0" t="s">
-        <v>254</v>
       </c>
       <c r="N42" s="0"/>
     </row>
@@ -2991,10 +2980,10 @@
         <v>261</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E43" s="6"/>
       <c r="F43" s="0" t="s">
@@ -3013,12 +3002,12 @@
         <v>266</v>
       </c>
       <c r="K43" s="0" t="s">
-        <v>252</v>
+        <v>42</v>
       </c>
       <c r="L43" s="0" t="s">
         <v>267</v>
       </c>
-      <c r="N43" s="11"/>
+      <c r="N43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
@@ -3028,10 +3017,10 @@
         <v>268</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E44" s="6"/>
       <c r="F44" s="0" t="s">
@@ -3050,10 +3039,10 @@
         <v>273</v>
       </c>
       <c r="K44" s="0" t="s">
-        <v>42</v>
+        <v>274</v>
       </c>
       <c r="L44" s="0" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="N44" s="0"/>
     </row>
@@ -3065,10 +3054,10 @@
         <v>275</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E45" s="6"/>
       <c r="F45" s="0" t="s">
@@ -3090,7 +3079,7 @@
         <v>281</v>
       </c>
       <c r="L45" s="0" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="N45" s="0"/>
     </row>
@@ -3099,35 +3088,35 @@
         <v>1</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E46" s="6"/>
       <c r="F46" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="G46" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="H46" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="I46" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="J46" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="K46" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="L46" s="0" t="s">
         <v>284</v>
-      </c>
-      <c r="H46" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="I46" s="0" t="s">
-        <v>286</v>
-      </c>
-      <c r="J46" s="0" t="s">
-        <v>287</v>
-      </c>
-      <c r="K46" s="0" t="s">
-        <v>288</v>
-      </c>
-      <c r="L46" s="0" t="s">
-        <v>289</v>
       </c>
       <c r="N46" s="0"/>
     </row>
@@ -3139,10 +3128,10 @@
         <v>290</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E47" s="6"/>
       <c r="F47" s="0" t="s">
@@ -3164,7 +3153,7 @@
         <v>296</v>
       </c>
       <c r="L47" s="0" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="N47" s="0"/>
     </row>
@@ -3173,35 +3162,35 @@
         <v>1</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E48" s="6"/>
       <c r="F48" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="J48" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="K48" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="L48" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="N48" s="0"/>
     </row>
@@ -3210,32 +3199,32 @@
         <v>1</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E49" s="6"/>
       <c r="F49" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="J49" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="K49" s="0" t="s">
-        <v>311</v>
+        <v>259</v>
       </c>
       <c r="L49" s="0" t="s">
         <v>312</v>
@@ -3253,7 +3242,7 @@
         <v>314</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E50" s="6"/>
       <c r="F50" s="0" t="s">
@@ -3275,7 +3264,7 @@
         <v>162</v>
       </c>
       <c r="L50" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="N50" s="0"/>
     </row>
@@ -3290,11 +3279,11 @@
         <v>321</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E51" s="6"/>
       <c r="F51" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="G51" s="0" t="s">
         <v>322</v>
@@ -3314,7 +3303,7 @@
       <c r="L51" s="0" t="s">
         <v>327</v>
       </c>
-      <c r="N51" s="9"/>
+      <c r="N51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
@@ -3327,7 +3316,7 @@
         <v>329</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E52" s="6"/>
       <c r="F52" s="0" t="s">
@@ -3351,7 +3340,7 @@
       <c r="L52" s="0" t="s">
         <v>336</v>
       </c>
-      <c r="N52" s="9"/>
+      <c r="N52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
@@ -3361,17 +3350,17 @@
         <v>337</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>321</v>
+        <v>338</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E53" s="6"/>
       <c r="F53" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>338</v>
+        <v>322</v>
       </c>
       <c r="H53" s="0" t="s">
         <v>323</v>
@@ -3398,14 +3387,14 @@
         <v>342</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="F54" s="0" t="s">
         <v>343</v>
-      </c>
-      <c r="F54" s="0" t="s">
-        <v>344</v>
       </c>
       <c r="G54" s="0" t="s">
         <v>345</v>
@@ -3423,11 +3412,11 @@
         <v>347</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D55" s="5"/>
       <c r="E55" s="6" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F55" s="0" t="s">
         <v>348</v>
@@ -3445,11 +3434,11 @@
         <v>350</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D56" s="6"/>
       <c r="E56" s="5" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F56" s="0" t="s">
         <v>351</v>
@@ -3467,11 +3456,11 @@
         <v>353</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D57" s="6"/>
       <c r="E57" s="5" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F57" s="0" t="s">
         <v>354</v>
@@ -3489,11 +3478,11 @@
         <v>356</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="5" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F58" s="0" t="s">
         <v>357</v>
@@ -3507,7 +3496,7 @@
       <c r="N58" s="0"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D32:D55 D2:D28">
+  <conditionalFormatting sqref="D50:D55 D2:D28 D32:D48">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"Y"</formula>
     </cfRule>
@@ -3515,7 +3504,7 @@
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E32:E55 E2:E28">
+  <conditionalFormatting sqref="E50:E55 E2:E28 E32:E48">
     <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>"DNP"</formula>
     </cfRule>
@@ -3559,6 +3548,19 @@
       <formula>"DNP"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D49">
+    <cfRule type="cellIs" priority="14" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E49">
+    <cfRule type="cellIs" priority="16" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"DNP"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>